<commit_message>
08-03-2025 changes  Frontend deployment
</commit_message>
<xml_diff>
--- a/excel/purchase_orders.xlsx
+++ b/excel/purchase_orders.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="26">
   <si>
     <t>Order ID</t>
   </si>
@@ -19,12 +19,18 @@
     <t>Product</t>
   </si>
   <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>Unit Price</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
     <t>Supplier</t>
   </si>
   <si>
-    <t>Ordered Quantity</t>
-  </si>
-  <si>
     <t>Order Date</t>
   </si>
   <si>
@@ -34,37 +40,55 @@
     <t>Payment Status</t>
   </si>
   <si>
-    <t>"67c75e26f99f7d1a983afa0c"</t>
-  </si>
-  <si>
-    <t>Advanced Paint Brush</t>
+    <t>"67ccdf22f25735bf5559c333"</t>
+  </si>
+  <si>
+    <t>Industrial Gloves</t>
+  </si>
+  <si>
+    <t>$5.00</t>
+  </si>
+  <si>
+    <t>$50.00</t>
   </si>
   <si>
     <t>Tech Supply Co.</t>
   </si>
   <si>
-    <t>2025-03-04</t>
-  </si>
-  <si>
-    <t>2025-03-09</t>
+    <t>2025-03-08</t>
+  </si>
+  <si>
+    <t>2025-03-15</t>
   </si>
   <si>
     <t>Pending</t>
   </si>
   <si>
-    <t>"67c75e26f99f7d1a983afa0d"</t>
-  </si>
-  <si>
-    <t>Heavy-Duty Gloves</t>
+    <t>Safety Glasses</t>
+  </si>
+  <si>
+    <t>$10.00</t>
+  </si>
+  <si>
+    <t>"67ccdf22f25735bf5559c336"</t>
+  </si>
+  <si>
+    <t>Hard Hat</t>
+  </si>
+  <si>
+    <t>$20.00</t>
+  </si>
+  <si>
+    <t>$300.00</t>
   </si>
   <si>
     <t>Manufacture Direct</t>
   </si>
   <si>
-    <t>2025-03-11</t>
-  </si>
-  <si>
-    <t>"67c760d12008a4e435498843"</t>
+    <t>"67ccdf22f25735bf5559c338"</t>
+  </si>
+  <si>
+    <t>$100.00</t>
   </si>
 </sst>
 </file>
@@ -441,15 +465,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:I5"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
-    <col min="1" max="1" width="25" customWidth="1"/>
-    <col min="2" max="3" width="20" customWidth="1"/>
-    <col min="4" max="7" width="15" customWidth="1"/>
+    <col min="1" max="1" width="20" customWidth="1"/>
+    <col min="2" max="2" width="30" customWidth="1"/>
+    <col min="3" max="5" width="15" customWidth="1"/>
+    <col min="6" max="6" width="25" customWidth="1"/>
+    <col min="7" max="9" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -471,74 +497,127 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>9</v>
       </c>
-      <c r="D2">
-        <v>30</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3">
+        <v>5</v>
+      </c>
+      <c r="D3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4">
+        <v>15</v>
+      </c>
+      <c r="D4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5">
         <v>10</v>
       </c>
-      <c r="F2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="D5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" t="s">
         <v>13</v>
       </c>
-      <c r="B3" t="s">
+      <c r="G5" t="s">
         <v>14</v>
       </c>
-      <c r="C3" t="s">
+      <c r="H5" t="s">
         <v>15</v>
       </c>
-      <c r="D3">
-        <v>50</v>
-      </c>
-      <c r="E3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" t="s">
+      <c r="I5" t="s">
         <v>16</v>
-      </c>
-      <c r="G3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4">
-        <v>2</v>
-      </c>
-      <c r="E4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G4" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>